<commit_message>
Fix build permissions for Render
</commit_message>
<xml_diff>
--- a/database/clientes.xlsx
+++ b/database/clientes.xlsx
@@ -427,7 +427,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ID-1751771630695-783</v>
+        <v>ID-1751811788755-80</v>
       </c>
       <c r="B2" t="str">
         <v>Matias Villagra</v>
@@ -442,7 +442,7 @@
         <v>5799989</v>
       </c>
       <c r="F2" t="str">
-        <v>2025-07-06T03:13:50.695Z</v>
+        <v>2025-07-06T14:23:08.755Z</v>
       </c>
       <c r="G2" t="str">
         <v>admin1</v>

</xml_diff>